<commit_message>
Added more data (G3)
</commit_message>
<xml_diff>
--- a/previous_results/Explanations.xlsx
+++ b/previous_results/Explanations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cahid\Documents\GitHub\Prisonner-s-Dilemma-Strategy-Evolution\previous_results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA517DA-EA28-4C96-AAEA-0BEE930BE7AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A44A2EF-78A1-44F4-A417-E62AB82A8F53}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6690" yWindow="2865" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="33">
   <si>
     <t>folder</t>
   </si>
@@ -447,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,6 +836,38 @@
         <v>32</v>
       </c>
     </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>32</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>1000000</v>
+      </c>
+      <c r="F14">
+        <v>500</v>
+      </c>
+      <c r="G14" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>